<commit_message>
FIXUP: Negative carbon cost sectors
1. Change CC: Carbon_costs.R script to allow for negative carbon costs
2. Change MAC curve allocations in Data cleaning: Market_parameterisation.R script to disallow 'Paper' from Forestry, everything from Agri
3. Alter Data cleaning: product classification spreadsheet to map 'sewage ...' to 'Water' sector instead of 'Waste Svcs'
</commit_message>
<xml_diff>
--- a/Data_cleaning/2_Financial/2c_Product_exposure/Input/Market_product_classification_EM.xlsx
+++ b/Data_cleaning/2_Financial/2c_Product_exposure/Input/Market_product_classification_EM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shyamal\Vivid Economics Ltd\171211HSB - Low Carbon Portfolio - Documents\6 - analysis\0 - Data cleaning\6 - Financial prod\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shyamal\Vivid Economics Ltd\171211HSB - Low Carbon Portfolio - Documents\6 - analysis\Data_cleaning\2_Financial\2c_Product_exposure\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="282" documentId="8_{81CE8ADD-4789-4B0C-817D-713ECBB34194}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{48A5AC8F-4F3D-4852-811F-F2B76FE1CFD4}"/>
+  <xr:revisionPtr revIDLastSave="285" documentId="8_{81CE8ADD-4789-4B0C-817D-713ECBB34194}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{38B11D83-718F-4CA8-B693-1B75D832C34E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="R1. Market product match" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,15 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'R1. Market product match'!$A$9:$D$3565</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -9682,7 +9690,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -9693,7 +9701,6 @@
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="35" borderId="0" xfId="42" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -10056,10 +10063,10 @@
   <dimension ref="A1:D3565"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="9" topLeftCell="C1586" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="9" topLeftCell="C3514" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1600" sqref="A1600"/>
+      <selection pane="bottomRight" activeCell="B3521" sqref="B3521"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16908,7 +16915,7 @@
       <c r="A605" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B605" s="8" t="s">
+      <c r="B605" s="2" t="s">
         <v>607</v>
       </c>
       <c r="C605" s="2" t="s">
@@ -17556,7 +17563,7 @@
       <c r="A662" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B662" s="8" t="s">
+      <c r="B662" s="2" t="s">
         <v>658</v>
       </c>
       <c r="C662" s="2" t="s">
@@ -18263,7 +18270,7 @@
         <v>708</v>
       </c>
       <c r="C724" s="2" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
     </row>
     <row r="725" spans="1:4" x14ac:dyDescent="0.3">
@@ -50416,7 +50423,7 @@
         <v>2926</v>
       </c>
       <c r="C3521" s="2" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3522" spans="1:3" x14ac:dyDescent="0.3">
@@ -50427,7 +50434,7 @@
         <v>2927</v>
       </c>
       <c r="C3522" s="2" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3523" spans="1:3" x14ac:dyDescent="0.3">
@@ -50908,7 +50915,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A9:D3565" xr:uid="{A6D60A50-187B-4979-9501-A1E6FA600206}">
-    <sortState ref="A10:D3565">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A10:D3565">
       <sortCondition ref="A9:A3565"/>
     </sortState>
   </autoFilter>
@@ -50922,6 +50929,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010071A458A34C1B804487783B2D6E744E74" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="db55914762f75c69a3f428beb16e5e78">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5fc07e1-684f-42dd-a9b9-4a385070eb2f" xmlns:ns3="40da89ef-49c0-40fe-8775-bed27f6d4e3e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3788be5c6e889f205c249745f37b3686" ns2:_="" ns3:_="">
     <xsd:import namespace="b5fc07e1-684f-42dd-a9b9-4a385070eb2f"/>
@@ -51112,46 +51134,46 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9385EFFF-1945-4F0A-BB1E-583479C3B5AA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBA3668C-65A9-4D35-9131-088D8D74D030}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40610A88-1C47-46DA-825C-BE2B4B759157}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="b5fc07e1-684f-42dd-a9b9-4a385070eb2f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="40da89ef-49c0-40fe-8775-bed27f6d4e3e"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="b5fc07e1-684f-42dd-a9b9-4a385070eb2f"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBA3668C-65A9-4D35-9131-088D8D74D030}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9385EFFF-1945-4F0A-BB1E-583479C3B5AA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b5fc07e1-684f-42dd-a9b9-4a385070eb2f"/>
+    <ds:schemaRef ds:uri="40da89ef-49c0-40fe-8775-bed27f6d4e3e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>